<commit_message>
Added the .bat file
</commit_message>
<xml_diff>
--- a/CONFIG/lists.xlsx
+++ b/CONFIG/lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ELNA\OCR_ELNA\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD6B967-DCB1-48A4-A98A-2B531C330664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3966E2F9-155B-4446-99CF-B21834A12117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nutricia" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="280">
   <si>
     <t>Imperativement garder les mêmes noms de colonnes</t>
   </si>
@@ -815,9 +815,6 @@
     <t>ZVPC0</t>
   </si>
   <si>
-    <t>analyse</t>
-  </si>
-  <si>
     <t>PAA4A</t>
   </si>
   <si>
@@ -863,7 +860,7 @@
     <t>Fatty Acids Profile-(Absolute &amp; Relative)-(w/o Fat Extr.)</t>
   </si>
   <si>
-    <t>code_lims</t>
+    <t>Denomination</t>
   </si>
 </sst>
 </file>
@@ -974,7 +971,7 @@
     <sortCondition ref="A1:A1048576"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{8EEC5650-4F60-4030-8EFB-927AA5E15102}" name="analyse"/>
+    <tableColumn id="1" xr3:uid="{8EEC5650-4F60-4030-8EFB-927AA5E15102}" name="Denomination"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -987,7 +984,7 @@
     <sortCondition ref="B1:B1048576"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2CC390DF-F2B3-4BAA-A19A-A28C665CC345}" name="code_lims"/>
+    <tableColumn id="1" xr3:uid="{2CC390DF-F2B3-4BAA-A19A-A28C665CC345}" name="Code"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1000,7 +997,7 @@
     <sortCondition ref="A1:A1048576"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{45AC102F-AFCC-4BE5-83B0-3A4616B78FF2}" name="analyse"/>
+    <tableColumn id="1" xr3:uid="{45AC102F-AFCC-4BE5-83B0-3A4616B78FF2}" name="Denomination"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1294,7 +1291,7 @@
   <dimension ref="A1:C269"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1305,10 +1302,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
       <c r="B1" t="s">
-        <v>280</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -3028,10 +3025,10 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B216" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
@@ -3428,34 +3425,34 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B266" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B267" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B268" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B269" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3472,9 +3469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15ACD5A-75CC-4B34-98C3-E10155F9E08B}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3483,57 +3478,57 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>